<commit_message>
added everything needed for future sea level predictions
</commit_message>
<xml_diff>
--- a/climatechangedata.xlsx
+++ b/climatechangedata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjdas\uofo-virt-data-pt-12-2021-u-b\final_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e42d87413de08d9/Desktop/bootcamp/resources/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125CA421-996F-408C-978F-2D9729631F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{125CA421-996F-408C-978F-2D9729631F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{286DA660-F4CB-46B7-BCDE-9E30D3D3E5A7}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{C0F098E5-2659-493F-AD87-3825EC2A0A5D}"/>
+    <workbookView xWindow="0" yWindow="2748" windowWidth="17280" windowHeight="8880" xr2:uid="{C0F098E5-2659-493F-AD87-3825EC2A0A5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,24 +442,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F31D490-C307-4009-A29E-98CE0504B800}">
   <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="1"/>
-    <col min="2" max="2" width="20.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="20.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.06640625" style="1"/>
+    <col min="7" max="7" width="28.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -485,7 +485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2020</v>
       </c>
@@ -512,7 +512,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2019</v>
       </c>
@@ -538,7 +538,7 @@
         <v>0.876</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2018</v>
       </c>
@@ -564,7 +564,7 @@
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2017</v>
       </c>
@@ -590,7 +590,7 @@
         <v>0.82199999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2016</v>
       </c>
@@ -616,7 +616,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2015</v>
       </c>
@@ -642,7 +642,7 @@
         <v>0.85799999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2014</v>
       </c>
@@ -668,7 +668,7 @@
         <v>0.64200000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2013</v>
       </c>
@@ -694,7 +694,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2012</v>
       </c>
@@ -720,7 +720,7 @@
         <v>0.44400000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2011</v>
       </c>
@@ -746,7 +746,7 @@
         <v>0.318</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2010</v>
       </c>
@@ -772,7 +772,7 @@
         <v>0.51600000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2009</v>
       </c>
@@ -798,7 +798,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2008</v>
       </c>
@@ -824,7 +824,7 @@
         <v>0.26400000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2007</v>
       </c>
@@ -850,7 +850,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2006</v>
       </c>
@@ -876,7 +876,7 @@
         <v>0.42599999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2005</v>
       </c>
@@ -902,7 +902,7 @@
         <v>0.42599999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2004</v>
       </c>
@@ -928,7 +928,7 @@
         <v>0.42599999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2003</v>
       </c>
@@ -954,7 +954,7 @@
         <v>0.46200000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2002</v>
       </c>
@@ -980,7 +980,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2001</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>0.35399999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2000</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1999</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1998</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>0.44400000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1997</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>0.35399999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1996</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>1995</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>0.17399999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1994</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1993</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1992</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1991</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>0.192</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>1990</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>0.246</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>1989</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>1988</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>0.13800000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>1987</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>1986</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>-4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>1985</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>-0.114</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>1984</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>-4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>1983</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>0.13800000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>1982</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>-6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>1981</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>-6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>1980</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>1979</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>1978</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>-0.186</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>1977</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>-7.8E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>1976</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>-0.36599999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>1975</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>-0.438</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>1974</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>-0.42</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>1973</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>1972</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>-0.186</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>1971</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>-0.51</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>1970</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>-0.29399999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>1969</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>-9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>1968</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>-0.38400000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>1967</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>-0.42</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>1966</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>-0.38400000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>1965</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>-0.47399999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>1964</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>-0.54600000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>1963</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>-0.27600000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>1962</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>-0.29399999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>1961</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>-0.27600000000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>1960</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>-0.312</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>1959</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>-0.29399999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>1958</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>-0.20399999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>1957</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>-0.222</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>1956</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>-0.56399999999999995</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>1955</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>-0.63600000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>1954</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>1953</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>-0.312</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>1952</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>-0.312</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>1951</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>-0.42</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>1950</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>-0.56399999999999995</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>1949</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>-0.56399999999999995</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>1948</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>-0.61799999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>1947</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>-0.54600000000000004</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>1946</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>-0.49199999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>1945</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>-2.4E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>1944</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>1943</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>-0.29399999999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>1942</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>-0.25800000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>1941</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>1940</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>1939</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>-0.49199999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>1938</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>1937</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>-0.47399999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>1936</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>-0.63600000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>1935</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>-0.70799999999999996</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>1934</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>-0.70799999999999996</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>1933</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>-0.79800000000000004</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>1932</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>-0.72599999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>1931</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>-0.58199999999999996</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>1930</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>-0.63600000000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>1929</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>-0.87</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>1928</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>-0.78</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>1927</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>-0.70799999999999996</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>1926</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>1925</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>-0.76200000000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>1924</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>-0.83399999999999996</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>1923</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>-0.81599999999999995</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>1922</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>-0.83399999999999996</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>1921</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>-0.74399999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>1920</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>-0.78</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>1919</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>-0.79800000000000004</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>1918</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>-0.72599999999999998</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>1917</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>-0.96</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>1916</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>-0.87</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>1915</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>-0.56399999999999995</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>1914</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>-0.69</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>1913</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>-0.94199999999999995</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>1912</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>-0.87</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>1911</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>-1.1220000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>1910</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>-1.1399999999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>1909</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>-1.1759999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>1908</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>-1.1040000000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>1907</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>-0.87</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>1906</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>-0.76200000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>1905</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>-0.79800000000000004</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>1904</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>-1.1579999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>1903</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>-1.014</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>1902</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>-0.76200000000000001</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>1901</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>-0.63600000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>1900</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>-0.438</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>1899</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>1898</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>-0.70799999999999996</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>1897</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>-0.42</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>1896</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>-0.33</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>1895</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>-0.56399999999999995</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>1894</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>-0.76200000000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>1893</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>-0.72599999999999998</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>1892</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>-0.65400000000000003</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>1891</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>-0.54600000000000004</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>1890</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>-0.81599999999999995</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>1889</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>-0.40200000000000002</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>1888</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>-0.40200000000000002</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>1887</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>-0.72599999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>1886</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>-0.67200000000000004</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>1885</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>-0.69</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>1884</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>-0.58199999999999996</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>1883</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>-0.45600000000000002</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>1882</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>-0.34799999999999998</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>1881</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>-0.33</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>1880</v>
       </c>

</xml_diff>